<commit_message>
Changes regarding the MTF tiers
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,7 +691,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -769,7 +769,7 @@
   <dimension ref="A1:AP2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,19 +940,19 @@
         <v>0.2</v>
       </c>
       <c r="M2">
-        <v>5.5</v>
+        <v>4.3</v>
       </c>
       <c r="N2">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="O2">
-        <v>0.8</v>
+        <v>0.83</v>
       </c>
       <c r="P2">
         <v>1.5</v>
       </c>
       <c r="Q2">
-        <v>0.08</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="R2">
         <v>2000</v>

</xml_diff>

<commit_message>
Updated the specs one scenario file and changed code so that it reads rural and urban elec ratios from the spreadsheet
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -10,15 +10,14 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioParameters" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsData" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib1" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="145621" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>Scenario</t>
   </si>
@@ -140,12 +139,27 @@
     <t>MaxGridExtensionDist</t>
   </si>
   <si>
+    <t>NewGridGenerationCapacityTimestepLimit</t>
+  </si>
+  <si>
     <t>ElecActual</t>
   </si>
   <si>
+    <t>Rural_elec_ratio</t>
+  </si>
+  <si>
+    <t>Urban_elec_ratio</t>
+  </si>
+  <si>
     <t>ElecModelled</t>
   </si>
   <si>
+    <t>urban_elec_ratio_modelled</t>
+  </si>
+  <si>
+    <t>rural_elec_ratio_modelled</t>
+  </si>
+  <si>
     <t>MinNightLights</t>
   </si>
   <si>
@@ -162,42 +176,6 @@
   </si>
   <si>
     <t>PopCutOffRoundTwo</t>
-  </si>
-  <si>
-    <t>Cap_Cost_grid</t>
-  </si>
-  <si>
-    <t>Cap_Cost_MG_PV</t>
-  </si>
-  <si>
-    <t>Cap_Cost_MG_DS</t>
-  </si>
-  <si>
-    <t>Cap_Cost_MG_WD</t>
-  </si>
-  <si>
-    <t>Cap_Cost_MG_HD</t>
-  </si>
-  <si>
-    <t>Cap_Cost_SA_PV</t>
-  </si>
-  <si>
-    <t>Cap_Cost_SA_DS</t>
-  </si>
-  <si>
-    <t>NewGridGenerationCapacityTimestepLimit</t>
-  </si>
-  <si>
-    <t>Rural_elec_ratio</t>
-  </si>
-  <si>
-    <t>Urban_elec_ratio</t>
-  </si>
-  <si>
-    <t>rural_elec_ratio</t>
-  </si>
-  <si>
-    <t>urban_elec_ratio</t>
   </si>
   <si>
     <t>Malawi</t>
@@ -273,13 +251,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -780,57 +761,52 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="8"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="12.5703125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="8.140625"/>
-    <col customWidth="1" max="5" min="5" width="3.85546875"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="12.5703125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="19.42578125"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="12.28515625"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" width="20"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" width="15.85546875"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" width="15.42578125"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" width="18.5703125"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" width="22.140625"/>
-    <col bestFit="1" customWidth="1" max="14" min="14" width="23"/>
-    <col bestFit="1" customWidth="1" max="15" min="15" width="14.7109375"/>
-    <col bestFit="1" customWidth="1" max="16" min="16" width="15.140625"/>
-    <col bestFit="1" customWidth="1" max="17" min="17" width="9.28515625"/>
-    <col bestFit="1" customWidth="1" max="18" min="18" width="26.85546875"/>
-    <col bestFit="1" customWidth="1" max="19" min="19" width="10.5703125"/>
-    <col bestFit="1" customWidth="1" max="20" min="20" width="11.5703125"/>
-    <col bestFit="1" customWidth="1" max="21" min="21" width="20.42578125"/>
-    <col bestFit="1" customWidth="1" max="22" min="22" width="21.140625"/>
-    <col bestFit="1" customWidth="1" max="23" min="23" width="10.140625"/>
-    <col bestFit="1" customWidth="1" max="24" min="24" width="13.42578125"/>
-    <col bestFit="1" customWidth="1" max="25" min="25" width="14.7109375"/>
-    <col bestFit="1" customWidth="1" max="26" min="26" width="11.28515625"/>
-    <col bestFit="1" customWidth="1" max="27" min="27" width="12.140625"/>
-    <col bestFit="1" customWidth="1" max="28" min="28" width="12.7109375"/>
-    <col bestFit="1" customWidth="1" max="30" min="29" width="20"/>
-    <col bestFit="1" customWidth="1" max="31" min="31" width="13.7109375"/>
-    <col bestFit="1" customWidth="1" max="32" min="32" width="17"/>
-    <col bestFit="1" customWidth="1" max="33" min="33" width="16.85546875"/>
-    <col bestFit="1" customWidth="1" max="34" min="34" width="18"/>
-    <col bestFit="1" customWidth="1" max="35" min="35" width="17.28515625"/>
-    <col bestFit="1" customWidth="1" max="36" min="36" width="16"/>
-    <col bestFit="1" customWidth="1" max="37" min="37" width="15.85546875"/>
-    <col bestFit="1" customWidth="1" max="38" min="38" width="40.28515625"/>
-    <col bestFit="1" customWidth="1" max="39" min="39" width="15.5703125"/>
-    <col bestFit="1" customWidth="1" max="40" min="40" width="16.42578125"/>
-    <col bestFit="1" customWidth="1" max="41" min="41" width="15.140625"/>
-    <col bestFit="1" customWidth="1" max="42" min="42" width="16.140625"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="8"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="2" width="12.5703125"/>
+    <col customWidth="1" max="3" min="3" style="2" width="9.140625"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="2" width="8.140625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="2" width="9.42578125"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="2" width="12.5703125"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="2" width="19.42578125"/>
+    <col bestFit="1" customWidth="1" max="8" min="8" style="2" width="12.28515625"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="2" width="20"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="2" width="15.85546875"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="2" width="15.42578125"/>
+    <col bestFit="1" customWidth="1" max="12" min="12" style="2" width="18.5703125"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" style="2" width="22.140625"/>
+    <col bestFit="1" customWidth="1" max="14" min="14" style="2" width="23"/>
+    <col bestFit="1" customWidth="1" max="15" min="15" style="2" width="14.7109375"/>
+    <col bestFit="1" customWidth="1" max="16" min="16" style="2" width="15.140625"/>
+    <col bestFit="1" customWidth="1" max="17" min="17" style="2" width="9.28515625"/>
+    <col bestFit="1" customWidth="1" max="18" min="18" style="2" width="26.85546875"/>
+    <col bestFit="1" customWidth="1" max="19" min="19" style="2" width="10.5703125"/>
+    <col bestFit="1" customWidth="1" max="20" min="20" style="2" width="11.5703125"/>
+    <col bestFit="1" customWidth="1" max="21" min="21" style="2" width="20.42578125"/>
+    <col bestFit="1" customWidth="1" max="22" min="22" style="2" width="21.140625"/>
+    <col bestFit="1" customWidth="1" max="23" min="23" style="2" width="40.28515625"/>
+    <col bestFit="1" customWidth="1" max="24" min="24" style="2" width="10.140625"/>
+    <col bestFit="1" customWidth="1" max="25" min="25" style="2" width="15.5703125"/>
+    <col bestFit="1" customWidth="1" max="26" min="26" style="2" width="16.42578125"/>
+    <col bestFit="1" customWidth="1" max="27" min="27" style="2" width="13.42578125"/>
+    <col bestFit="1" customWidth="1" max="28" min="28" style="2" width="26.140625"/>
+    <col bestFit="1" customWidth="1" max="29" min="29" style="2" width="25"/>
+    <col bestFit="1" customWidth="1" max="30" min="30" style="2" width="14.7109375"/>
+    <col bestFit="1" customWidth="1" max="31" min="31" style="2" width="11.28515625"/>
+    <col bestFit="1" customWidth="1" max="32" min="32" style="2" width="12.140625"/>
+    <col bestFit="1" customWidth="1" max="33" min="33" style="2" width="12.7109375"/>
+    <col bestFit="1" customWidth="1" max="35" min="34" style="2" width="20"/>
+    <col customWidth="1" max="16384" min="36" style="2" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:35">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -936,127 +912,100 @@
       <c r="AI1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42">
-      <c r="A2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="C2" s="2" t="n">
         <v>2018</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" s="2" t="n">
         <v>18620000</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" s="2" t="n">
         <v>0.17</v>
       </c>
-      <c r="H2" t="n">
-        <v>2858.003227632393</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.147018428409968</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="H2" s="2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J2" s="2" t="n">
         <v>30000000</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2" s="2" t="n">
         <v>26600000</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2" s="2" t="n">
         <v>0.2</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2" s="2" t="n">
         <v>4.3</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2" s="2" t="n">
         <v>4.5</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2" s="2" t="n">
         <v>0.83</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2" s="2" t="n">
         <v>1.5</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2" s="2" t="n">
         <v>0.076</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2" s="2" t="n">
         <v>1874</v>
       </c>
-      <c r="S2" t="n">
+      <c r="S2" s="2" t="n">
         <v>0.1</v>
       </c>
-      <c r="T2" t="n">
+      <c r="T2" s="2" t="n">
         <v>0.85</v>
       </c>
-      <c r="U2" t="n">
+      <c r="U2" s="2" t="n">
         <v>0.1</v>
       </c>
-      <c r="V2" t="n">
-        <v>70</v>
-      </c>
-      <c r="W2" t="n">
+      <c r="V2" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="W2" s="2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="X2" s="2" t="n">
         <v>0.11</v>
       </c>
-      <c r="Y2" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z2" t="n">
+      <c r="Y2" s="2" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="Z2" s="2" t="n">
+        <v>0.492</v>
+      </c>
+      <c r="AD2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AF2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AG2" s="2" t="n">
         <v>0.5</v>
       </c>
-      <c r="AC2" t="n">
-        <v>6140.790349047872</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>6000</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>4300</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.492</v>
+      <c r="AH2" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AI2" s="2" t="n">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -1070,7 +1019,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1078,140 +1027,119 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:42">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:35">
+      <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="B2" t="s">
         <v>54</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
       </c>
       <c r="C2" t="n">
         <v>2018</v>
@@ -1229,7 +1157,7 @@
         <v>0.17</v>
       </c>
       <c r="H2" t="n">
-        <v>2858.003227632393</v>
+        <v>2000</v>
       </c>
       <c r="I2" t="n">
         <v>0.1400786370592801</v>
@@ -1271,312 +1199,46 @@
         <v>0.1</v>
       </c>
       <c r="V2" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="W2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="X2" t="n">
         <v>0.11</v>
       </c>
-      <c r="X2" t="n">
+      <c r="Y2" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.492</v>
+      </c>
+      <c r="AA2" t="n">
         <v>0.237378741558234</v>
       </c>
-      <c r="Y2" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z2" t="n">
+      <c r="AB2" t="n">
+        <v>0.6216619422975829</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.2829673231553027</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
         <v>1</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AF2" t="n">
         <v>1</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AG2" t="n">
         <v>0.5</v>
       </c>
-      <c r="AC2" t="n">
-        <v>6140.790349047872</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>6000</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>4300</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.492</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.7503283795844339</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.2117012459425293</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AP2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:42">
-      <c r="A1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AM1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AN1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AP1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42">
-      <c r="A2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2018</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2030</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>18620000</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2858.003227632393</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.1400786370592801</v>
-      </c>
-      <c r="J2" t="n">
-        <v>30000000</v>
-      </c>
-      <c r="K2" t="n">
-        <v>26600000</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M2" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="N2" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1874</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="V2" t="n">
-        <v>70</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.237378741558234</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>6140.790349047872</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>6000</v>
-      </c>
-      <c r="AE2" t="s"/>
-      <c r="AF2" t="n">
-        <v>4300</v>
-      </c>
-      <c r="AG2" t="s"/>
-      <c r="AH2" t="s"/>
-      <c r="AI2" t="s"/>
-      <c r="AJ2" t="s"/>
-      <c r="AK2" t="s"/>
-      <c r="AL2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.492</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.7503283795844339</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.2117012459425293</v>
+      <c r="AH2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes on the calibration process
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alekor\Desktop\GithubClones\GEP-Working-dir\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioInfo" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioParameters" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsData" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
+    <sheet name="ScenarioParameters" sheetId="2" r:id="rId2"/>
+    <sheet name="SpecsData" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Scenario</t>
   </si>
@@ -154,12 +158,6 @@
     <t>ElecModelled</t>
   </si>
   <si>
-    <t>urban_elec_ratio_modelled</t>
-  </si>
-  <si>
-    <t>rural_elec_ratio_modelled</t>
-  </si>
-  <si>
     <t>MinNightLights</t>
   </si>
   <si>
@@ -182,42 +180,44 @@
   </si>
   <si>
     <t>mw</t>
+  </si>
+  <si>
+    <t>urban_elec_ratio</t>
+  </si>
+  <si>
+    <t>rural_elec_ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -240,36 +240,35 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -535,31 +534,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="8"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="17"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="32.140625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="26"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="28"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="10.5703125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="10.85546875"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="22.140625"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" width="20.42578125"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -588,64 +583,60 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="10.7109375"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="14.42578125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="13.7109375"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="17.28515625"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="10.7109375"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" width="16.5703125"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" width="19.5703125"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -674,139 +665,136 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>0.4</v>
       </c>
-      <c r="F2" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="F2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G2">
         <v>4300</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>0.83</v>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="n">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>4</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>0.8</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>0.08</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>5500</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>1.5</v>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="n">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>6</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AI6" sqref="AI6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="8"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="2" width="12.5703125"/>
-    <col customWidth="1" max="3" min="3" style="2" width="9.140625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="2" width="8.140625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="2" width="9.42578125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="2" width="12.5703125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="2" width="19.42578125"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="2" width="12.28515625"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="2" width="20"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="2" width="15.85546875"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="2" width="15.42578125"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="2" width="18.5703125"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="2" width="22.140625"/>
-    <col bestFit="1" customWidth="1" max="14" min="14" style="2" width="23"/>
-    <col bestFit="1" customWidth="1" max="15" min="15" style="2" width="14.7109375"/>
-    <col bestFit="1" customWidth="1" max="16" min="16" style="2" width="15.140625"/>
-    <col bestFit="1" customWidth="1" max="17" min="17" style="2" width="9.28515625"/>
-    <col bestFit="1" customWidth="1" max="18" min="18" style="2" width="26.85546875"/>
-    <col bestFit="1" customWidth="1" max="19" min="19" style="2" width="10.5703125"/>
-    <col bestFit="1" customWidth="1" max="20" min="20" style="2" width="11.5703125"/>
-    <col bestFit="1" customWidth="1" max="21" min="21" style="2" width="20.42578125"/>
-    <col bestFit="1" customWidth="1" max="22" min="22" style="2" width="21.140625"/>
-    <col bestFit="1" customWidth="1" max="23" min="23" style="2" width="40.28515625"/>
-    <col bestFit="1" customWidth="1" max="24" min="24" style="2" width="10.140625"/>
-    <col bestFit="1" customWidth="1" max="25" min="25" style="2" width="15.5703125"/>
-    <col bestFit="1" customWidth="1" max="26" min="26" style="2" width="16.42578125"/>
-    <col bestFit="1" customWidth="1" max="27" min="27" style="2" width="13.42578125"/>
-    <col bestFit="1" customWidth="1" max="28" min="28" style="2" width="26.140625"/>
-    <col bestFit="1" customWidth="1" max="29" min="29" style="2" width="25"/>
-    <col bestFit="1" customWidth="1" max="30" min="30" style="2" width="14.7109375"/>
-    <col bestFit="1" customWidth="1" max="31" min="31" style="2" width="11.28515625"/>
-    <col bestFit="1" customWidth="1" max="32" min="32" style="2" width="12.140625"/>
-    <col bestFit="1" customWidth="1" max="33" min="33" style="2" width="12.7109375"/>
-    <col bestFit="1" customWidth="1" max="35" min="34" style="2" width="20"/>
-    <col customWidth="1" max="16384" min="36" style="2" width="9.140625"/>
+    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="41" width="9.140625" style="2" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -889,359 +877,126 @@
         <v>44</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AH1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:35">
-      <c r="A2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>2018</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="2">
         <v>2030</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="2">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <v>18620000</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="2">
         <v>0.17</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="2">
         <v>2000</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="2">
         <v>30000000</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="2">
         <v>26600000</v>
       </c>
-      <c r="L2" s="2" t="n">
+      <c r="L2" s="2">
         <v>0.2</v>
       </c>
-      <c r="M2" s="2" t="n">
+      <c r="M2" s="2">
         <v>4.3</v>
       </c>
-      <c r="N2" s="2" t="n">
+      <c r="N2" s="2">
         <v>4.5</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="O2" s="2">
         <v>0.83</v>
       </c>
-      <c r="P2" s="2" t="n">
+      <c r="P2" s="2">
         <v>1.5</v>
       </c>
-      <c r="Q2" s="2" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="R2" s="2" t="n">
+      <c r="Q2" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="R2" s="2">
         <v>1874</v>
       </c>
-      <c r="S2" s="2" t="n">
+      <c r="S2" s="2">
         <v>0.1</v>
       </c>
-      <c r="T2" s="2" t="n">
+      <c r="T2" s="2">
         <v>0.85</v>
       </c>
-      <c r="U2" s="2" t="n">
+      <c r="U2" s="2">
         <v>0.1</v>
       </c>
-      <c r="V2" s="2" t="n">
+      <c r="V2" s="2">
         <v>50</v>
       </c>
-      <c r="W2" s="2" t="n">
+      <c r="W2" s="2">
         <v>1500</v>
       </c>
-      <c r="X2" s="2" t="n">
+      <c r="X2" s="2">
         <v>0.11</v>
       </c>
-      <c r="Y2" s="2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="Z2" s="2" t="n">
-        <v>0.492</v>
-      </c>
-      <c r="AD2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="2" t="n">
+      <c r="Y2" s="2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="2">
         <v>1</v>
       </c>
-      <c r="AF2" s="2" t="n">
+      <c r="AF2" s="2">
         <v>1</v>
       </c>
-      <c r="AG2" s="2" t="n">
+      <c r="AG2" s="2">
         <v>0.5</v>
       </c>
-      <c r="AH2" s="2" t="n">
+      <c r="AH2" s="2">
         <v>5000</v>
       </c>
-      <c r="AI2" s="2" t="n">
+      <c r="AI2" s="2">
         <v>10000</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AI2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:35">
-      <c r="A1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2018</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2030</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>18620000</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.1400786370592801</v>
-      </c>
-      <c r="J2" t="n">
-        <v>30000000</v>
-      </c>
-      <c r="K2" t="n">
-        <v>26600000</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M2" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="N2" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1874</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="V2" t="n">
-        <v>50</v>
-      </c>
-      <c r="W2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.492</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.237378741558234</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0.6216619422975829</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.2829673231553027</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Latest update before elec code is changed
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -10,6 +10,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioParameters" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsData" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib3" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1245,4 +1248,703 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AI2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:35">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>18620000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.1609394603523363</v>
+      </c>
+      <c r="J2" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="K2" t="n">
+        <v>26600000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="N2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1874</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="V2" t="n">
+        <v>50</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.492</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.1283181294047265</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1.338921625438018</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.02335669498174712</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AI2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:35">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>18620000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.1609394603523363</v>
+      </c>
+      <c r="J2" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="K2" t="n">
+        <v>26600000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="N2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1874</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="V2" t="n">
+        <v>50</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.492</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.1283181294047265</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1.453444456925703</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.320394447286111</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AI2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:35">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2018</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2030</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>18620000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.1609394603523363</v>
+      </c>
+      <c r="J2" t="n">
+        <v>30000000</v>
+      </c>
+      <c r="K2" t="n">
+        <v>26600000</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M2" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="N2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1874</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="V2" t="n">
+        <v>50</v>
+      </c>
+      <c r="W2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.492</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.1194181269674673</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1.346468636883841</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.3163577515461272</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Identifying curently electrified pop so that it matches urban/rural statistics update
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,8 +11,6 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsData" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib2" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib3" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -157,10 +155,10 @@
     <t>ElecModelled</t>
   </si>
   <si>
-    <t>urban_elec_ratio</t>
-  </si>
-  <si>
-    <t>rural_elec_ratio</t>
+    <t>urban_elec_ratio_modelled</t>
+  </si>
+  <si>
+    <t>rural_elec_ratio_modelled</t>
   </si>
   <si>
     <t>MinNightLights</t>
@@ -545,7 +543,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -766,8 +764,8 @@
   </sheetPr>
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD7" sqref="AD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -799,15 +797,15 @@
     <col bestFit="1" customWidth="1" max="25" min="25" style="2" width="15.5703125"/>
     <col bestFit="1" customWidth="1" max="26" min="26" style="2" width="16.42578125"/>
     <col bestFit="1" customWidth="1" max="27" min="27" style="2" width="13.42578125"/>
-    <col bestFit="1" customWidth="1" max="28" min="28" style="2" width="26.140625"/>
-    <col bestFit="1" customWidth="1" max="29" min="29" style="2" width="25"/>
+    <col customWidth="1" max="28" min="28" style="2" width="12.140625"/>
+    <col customWidth="1" max="29" min="29" style="2" width="12.7109375"/>
     <col bestFit="1" customWidth="1" max="30" min="30" style="2" width="14.7109375"/>
     <col bestFit="1" customWidth="1" max="31" min="31" style="2" width="11.28515625"/>
     <col bestFit="1" customWidth="1" max="32" min="32" style="2" width="12.140625"/>
     <col bestFit="1" customWidth="1" max="33" min="33" style="2" width="12.7109375"/>
     <col bestFit="1" customWidth="1" max="35" min="34" style="2" width="20"/>
-    <col customWidth="1" max="41" min="36" style="2" width="9.140625"/>
-    <col customWidth="1" max="16384" min="42" style="2" width="9.140625"/>
+    <col customWidth="1" max="44" min="36" style="2" width="9.140625"/>
+    <col customWidth="1" max="16384" min="45" style="2" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -1218,13 +1216,13 @@
         <v>0.492</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.1201896909166762</v>
+        <v>0.11</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.7963675370694817</v>
+        <v>0.5104112205648693</v>
       </c>
       <c r="AC2" t="n">
-        <v>88.50793832230626</v>
+        <v>0.0331974777603167</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -1451,479 +1449,13 @@
         <v>0.492</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.1283181294047265</v>
+        <v>0.11</v>
       </c>
       <c r="AB2" t="n">
-        <v>1.338921625438018</v>
+        <v>0.5104112205648695</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.02335669498174712</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AI2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:35">
-      <c r="A1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2018</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2030</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>18620000</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.1609394603523363</v>
-      </c>
-      <c r="J2" t="n">
-        <v>30000000</v>
-      </c>
-      <c r="K2" t="n">
-        <v>26600000</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M2" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="N2" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1874</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="V2" t="n">
-        <v>50</v>
-      </c>
-      <c r="W2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.492</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.1283181294047265</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>1.453444456925703</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.320394447286111</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>5000</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AI2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:35">
-      <c r="A1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2018</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2030</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="n">
-        <v>18620000</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="H2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.1609394603523363</v>
-      </c>
-      <c r="J2" t="n">
-        <v>30000000</v>
-      </c>
-      <c r="K2" t="n">
-        <v>26600000</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M2" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="N2" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.83</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1874</v>
-      </c>
-      <c r="S2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="V2" t="n">
-        <v>50</v>
-      </c>
-      <c r="W2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.492</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.1194181269674673</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>1.346468636883841</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.3163577515461272</v>
+        <v>0.0331974777603167</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
New updated on calibration, regarding currently electrified settlements
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -543,7 +543,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -764,7 +764,7 @@
   </sheetPr>
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
@@ -804,8 +804,8 @@
     <col bestFit="1" customWidth="1" max="32" min="32" style="2" width="12.140625"/>
     <col bestFit="1" customWidth="1" max="33" min="33" style="2" width="12.7109375"/>
     <col bestFit="1" customWidth="1" max="35" min="34" style="2" width="20"/>
-    <col customWidth="1" max="44" min="36" style="2" width="9.140625"/>
-    <col customWidth="1" max="16384" min="45" style="2" width="9.140625"/>
+    <col customWidth="1" max="47" min="36" style="2" width="9.140625"/>
+    <col customWidth="1" max="16384" min="48" style="2" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -1216,10 +1216,10 @@
         <v>0.492</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.11</v>
+        <v>0.1100000000000001</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.5104112205648693</v>
+        <v>0.5104112205648695</v>
       </c>
       <c r="AC2" t="n">
         <v>0.0331974777603167</v>

</xml_diff>

<commit_message>
A few changes on lilitation application function and some TODOs here and there
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alekor\Desktop\GithubClones\GEP-Working-dir\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioInfo" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioParameters" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsData" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecsDataCalib1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
+    <sheet name="ScenarioParameters" sheetId="2" r:id="rId2"/>
+    <sheet name="SpecsData" sheetId="3" r:id="rId3"/>
+    <sheet name="SpecsDataCalib" sheetId="4" r:id="rId4"/>
+    <sheet name="SpecsDataCalib1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
   <si>
     <t>Scenario</t>
   </si>
@@ -188,31 +193,33 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -242,35 +249,52 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -536,31 +560,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="8"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="17"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="32.140625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="26"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="28"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="10.5703125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="10.85546875"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="22.140625"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" width="20.42578125"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,64 +609,60 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="2" min="2" width="10.7109375"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="14.42578125"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="13.7109375"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="17.28515625"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="10.7109375"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" width="16.5703125"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" width="19.5703125"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -675,140 +691,136 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <v>4</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>0.4</v>
       </c>
-      <c r="F2" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="F2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G2">
         <v>4300</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>0.83</v>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="n">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>4</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>0.8</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>0.08</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>5500</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>1.5</v>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="n">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>6</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="8"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="2" width="12.5703125"/>
-    <col customWidth="1" max="3" min="3" style="2" width="9.140625"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="2" width="8.140625"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="2" width="9.42578125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="2" width="12.5703125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="2" width="19.42578125"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" style="2" width="12.28515625"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="2" width="20"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="2" width="15.85546875"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="2" width="15.42578125"/>
-    <col bestFit="1" customWidth="1" max="12" min="12" style="2" width="18.5703125"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="2" width="22.140625"/>
-    <col bestFit="1" customWidth="1" max="14" min="14" style="2" width="23"/>
-    <col bestFit="1" customWidth="1" max="15" min="15" style="2" width="14.7109375"/>
-    <col bestFit="1" customWidth="1" max="16" min="16" style="2" width="15.140625"/>
-    <col bestFit="1" customWidth="1" max="17" min="17" style="2" width="9.28515625"/>
-    <col bestFit="1" customWidth="1" max="18" min="18" style="2" width="26.85546875"/>
-    <col bestFit="1" customWidth="1" max="19" min="19" style="2" width="10.5703125"/>
-    <col bestFit="1" customWidth="1" max="20" min="20" style="2" width="11.5703125"/>
-    <col bestFit="1" customWidth="1" max="21" min="21" style="2" width="20.42578125"/>
-    <col bestFit="1" customWidth="1" max="22" min="22" style="2" width="21.140625"/>
-    <col bestFit="1" customWidth="1" max="23" min="23" style="2" width="40.28515625"/>
-    <col bestFit="1" customWidth="1" max="24" min="24" style="2" width="10.140625"/>
-    <col bestFit="1" customWidth="1" max="25" min="25" style="2" width="15.5703125"/>
-    <col bestFit="1" customWidth="1" max="26" min="26" style="2" width="16.42578125"/>
-    <col bestFit="1" customWidth="1" max="27" min="27" style="2" width="13.42578125"/>
-    <col customWidth="1" max="28" min="28" style="2" width="12.140625"/>
-    <col customWidth="1" max="29" min="29" style="2" width="12.7109375"/>
-    <col bestFit="1" customWidth="1" max="30" min="30" style="2" width="14.7109375"/>
-    <col bestFit="1" customWidth="1" max="31" min="31" style="2" width="11.28515625"/>
-    <col bestFit="1" customWidth="1" max="32" min="32" style="2" width="12.140625"/>
-    <col bestFit="1" customWidth="1" max="33" min="33" style="2" width="12.7109375"/>
-    <col bestFit="1" customWidth="1" max="35" min="34" style="2" width="20"/>
-    <col customWidth="1" max="47" min="36" style="2" width="9.140625"/>
-    <col customWidth="1" max="16384" min="48" style="2" width="9.140625"/>
+    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.140625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" style="2" customWidth="1"/>
+    <col min="30" max="30" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="48" width="9.140625" style="2" customWidth="1"/>
+    <col min="49" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -915,121 +927,115 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="2">
         <v>2018</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="2">
         <v>2030</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="2">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="2">
         <v>18620000</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="2">
         <v>0.17</v>
       </c>
-      <c r="H2" s="2" t="n">
+      <c r="H2" s="2">
         <v>2000</v>
       </c>
-      <c r="J2" s="2" t="n">
+      <c r="J2" s="2">
         <v>30000000</v>
       </c>
-      <c r="K2" s="2" t="n">
+      <c r="K2" s="2">
         <v>26600000</v>
       </c>
-      <c r="L2" s="2" t="n">
+      <c r="L2" s="2">
         <v>0.2</v>
       </c>
-      <c r="M2" s="2" t="n">
+      <c r="M2" s="2">
         <v>4.3</v>
       </c>
-      <c r="N2" s="2" t="n">
+      <c r="N2" s="2">
         <v>4.5</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="O2" s="2">
         <v>0.83</v>
       </c>
-      <c r="P2" s="2" t="n">
+      <c r="P2" s="2">
         <v>1.5</v>
       </c>
-      <c r="Q2" s="2" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="R2" s="2" t="n">
+      <c r="Q2" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="R2" s="2">
         <v>1874</v>
       </c>
-      <c r="S2" s="2" t="n">
+      <c r="S2" s="2">
         <v>0.1</v>
       </c>
-      <c r="T2" s="2" t="n">
+      <c r="T2" s="2">
         <v>0.85</v>
       </c>
-      <c r="U2" s="2" t="n">
+      <c r="U2" s="2">
         <v>0.1</v>
       </c>
-      <c r="V2" s="2" t="n">
+      <c r="V2" s="2">
         <v>50</v>
       </c>
-      <c r="W2" s="2" t="n">
+      <c r="W2" s="2">
         <v>1500</v>
       </c>
-      <c r="X2" s="2" t="n">
+      <c r="X2" s="2">
         <v>0.11</v>
       </c>
-      <c r="Y2" s="2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="Z2" s="2" t="n">
-        <v>0.492</v>
-      </c>
-      <c r="AD2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="2" t="n">
+      <c r="Y2" s="2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="2">
         <v>1</v>
       </c>
-      <c r="AF2" s="2" t="n">
+      <c r="AF2" s="2">
         <v>1</v>
       </c>
-      <c r="AG2" s="2" t="n">
+      <c r="AG2" s="2">
         <v>0.5</v>
       </c>
-      <c r="AH2" s="2" t="n">
+      <c r="AH2" s="2">
         <v>5000</v>
       </c>
-      <c r="AI2" s="2" t="n">
+      <c r="AI2" s="2">
         <v>10000</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1136,133 +1142,127 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>2018</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>2030</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>5</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>18620000</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>0.17</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>2000</v>
       </c>
-      <c r="I2" t="n">
-        <v>0.1609394603523363</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="I2">
+        <v>0.16093946035233631</v>
+      </c>
+      <c r="J2">
         <v>30000000</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2">
         <v>26600000</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>0.2</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>4.3</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>4.5</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>0.83</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2">
         <v>1.5</v>
       </c>
-      <c r="Q2" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="R2" t="n">
+      <c r="Q2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="R2">
         <v>1874</v>
       </c>
-      <c r="S2" t="n">
+      <c r="S2">
         <v>0.1</v>
       </c>
-      <c r="T2" t="n">
+      <c r="T2">
         <v>0.85</v>
       </c>
-      <c r="U2" t="n">
+      <c r="U2">
         <v>0.1</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V2">
         <v>50</v>
       </c>
-      <c r="W2" t="n">
+      <c r="W2">
         <v>1500</v>
       </c>
-      <c r="X2" t="n">
+      <c r="X2">
         <v>0.11</v>
       </c>
-      <c r="Y2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.492</v>
-      </c>
-      <c r="AA2" t="n">
+      <c r="Y2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="Z2">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="AA2">
         <v>0.1100000000000001</v>
       </c>
-      <c r="AB2" t="n">
-        <v>0.5104112205648695</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.0331974777603167</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
+      <c r="AB2">
+        <v>0.51041122056486954</v>
+      </c>
+      <c r="AC2">
+        <v>3.3197477760316702E-2</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
         <v>1</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2">
         <v>1</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG2">
         <v>0.5</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AH2">
         <v>5000</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AI2">
         <v>10000</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1369,114 +1369,114 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>2018</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>2030</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>5</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>18620000</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>0.17</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>2000</v>
       </c>
-      <c r="I2" t="n">
-        <v>0.1609394603523363</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="I2">
+        <v>0.16093946035233631</v>
+      </c>
+      <c r="J2">
         <v>30000000</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2">
         <v>26600000</v>
       </c>
-      <c r="L2" t="n">
+      <c r="L2">
         <v>0.2</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>4.3</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>4.5</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>0.83</v>
       </c>
-      <c r="P2" t="n">
+      <c r="P2">
         <v>1.5</v>
       </c>
-      <c r="Q2" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="R2" t="n">
+      <c r="Q2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="R2">
         <v>1874</v>
       </c>
-      <c r="S2" t="n">
+      <c r="S2">
         <v>0.1</v>
       </c>
-      <c r="T2" t="n">
+      <c r="T2">
         <v>0.85</v>
       </c>
-      <c r="U2" t="n">
+      <c r="U2">
         <v>0.1</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V2">
         <v>50</v>
       </c>
-      <c r="W2" t="n">
+      <c r="W2">
         <v>1500</v>
       </c>
-      <c r="X2" t="n">
+      <c r="X2">
         <v>0.11</v>
       </c>
-      <c r="Y2" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.492</v>
-      </c>
-      <c r="AA2" t="n">
+      <c r="Y2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="Z2">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="AA2">
         <v>0.11</v>
       </c>
-      <c r="AB2" t="n">
-        <v>0.5104112205648695</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.0331974777603167</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="n">
+      <c r="AB2">
+        <v>0.51041122056486954</v>
+      </c>
+      <c r="AC2">
+        <v>3.3197477760316702E-2</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
         <v>1</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2">
         <v>1</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG2">
         <v>0.5</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AH2">
         <v>5000</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AI2">
         <v>10000</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Many updates: timestep deleted from specs, level on PV cost updated, #RUN_PARAM introduced
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
   <si>
     <t>Scenario</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Grid_electricity_generation_cost</t>
   </si>
   <si>
-    <t>SA_PV_cost</t>
-  </si>
-  <si>
     <t>Diesel_price</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
     <t>GridGenerationCost</t>
   </si>
   <si>
-    <t>SA_PV_Cost</t>
-  </si>
-  <si>
     <t>DieselPrice</t>
   </si>
   <si>
@@ -91,9 +85,6 @@
     <t>EndYEar</t>
   </si>
   <si>
-    <t>TimeStep</t>
-  </si>
-  <si>
     <t>PopStartYear</t>
   </si>
   <si>
@@ -188,6 +179,12 @@
   </si>
   <si>
     <t>mw</t>
+  </si>
+  <si>
+    <t>PV_cost_adjust</t>
+  </si>
+  <si>
+    <t>PV_Cost_adjust</t>
   </si>
 </sst>
 </file>
@@ -563,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -597,16 +594,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -647,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,38 +654,39 @@
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -711,7 +709,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="G2">
-        <v>4300</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>0.83</v>
@@ -743,7 +741,7 @@
         <v>0.08</v>
       </c>
       <c r="G3">
-        <v>5500</v>
+        <v>1.25</v>
       </c>
       <c r="H3">
         <v>1.5</v>
@@ -774,10 +772,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,153 +784,149 @@
     <col min="2" max="2" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.140625" style="2" customWidth="1"/>
-    <col min="29" max="29" width="12.7109375" style="2" customWidth="1"/>
-    <col min="30" max="30" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="48" width="9.140625" style="2" customWidth="1"/>
-    <col min="49" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="5" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="12.7109375" style="2" customWidth="1"/>
+    <col min="29" max="29" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="49" width="9.140625" style="2" customWidth="1"/>
+    <col min="50" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="C2" s="2">
         <v>2018</v>
@@ -941,84 +935,81 @@
         <v>2030</v>
       </c>
       <c r="E2" s="2">
-        <v>5</v>
+        <v>18620000</v>
       </c>
       <c r="F2" s="2">
-        <v>18620000</v>
+        <v>0.17</v>
       </c>
       <c r="G2" s="2">
-        <v>0.17</v>
-      </c>
-      <c r="H2" s="2">
         <v>2000</v>
       </c>
+      <c r="I2" s="2">
+        <v>30000000</v>
+      </c>
       <c r="J2" s="2">
-        <v>30000000</v>
+        <v>26600000</v>
       </c>
       <c r="K2" s="2">
-        <v>26600000</v>
+        <v>0.2</v>
       </c>
       <c r="L2" s="2">
-        <v>0.2</v>
+        <v>4.3</v>
       </c>
       <c r="M2" s="2">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="N2" s="2">
-        <v>4.5</v>
+        <v>0.83</v>
       </c>
       <c r="O2" s="2">
-        <v>0.83</v>
+        <v>1.5</v>
       </c>
       <c r="P2" s="2">
-        <v>1.5</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="Q2" s="2">
-        <v>7.5999999999999998E-2</v>
+        <v>1874</v>
       </c>
       <c r="R2" s="2">
-        <v>1874</v>
+        <v>0.1</v>
       </c>
       <c r="S2" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="T2" s="2">
         <v>0.1</v>
       </c>
-      <c r="T2" s="2">
-        <v>0.85</v>
-      </c>
       <c r="U2" s="2">
-        <v>0.1</v>
+        <v>50</v>
       </c>
       <c r="V2" s="2">
-        <v>50</v>
+        <v>1500</v>
       </c>
       <c r="W2" s="2">
-        <v>1500</v>
+        <v>0.11</v>
       </c>
       <c r="X2" s="2">
-        <v>0.11</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="Y2" s="2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="Z2" s="2">
         <v>0.49199999999999999</v>
       </c>
+      <c r="AC2" s="2">
+        <v>0</v>
+      </c>
       <c r="AD2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE2" s="2">
         <v>1</v>
       </c>
       <c r="AF2" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AG2" s="2">
-        <v>0.5</v>
+        <v>5000</v>
       </c>
       <c r="AH2" s="2">
-        <v>5000</v>
-      </c>
-      <c r="AI2" s="2">
         <v>10000</v>
       </c>
     </row>
@@ -1029,125 +1020,124 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>50</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="B2" t="s">
         <v>51</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
       </c>
       <c r="C2">
         <v>2018</v>
@@ -1156,96 +1146,93 @@
         <v>2030</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>18620000</v>
       </c>
       <c r="F2">
-        <v>18620000</v>
+        <v>0.17</v>
       </c>
       <c r="G2">
-        <v>0.17</v>
+        <v>2000</v>
       </c>
       <c r="H2">
-        <v>2000</v>
+        <v>0.16093946035233631</v>
       </c>
       <c r="I2">
-        <v>0.16093946035233631</v>
+        <v>30000000</v>
       </c>
       <c r="J2">
-        <v>30000000</v>
+        <v>26600000</v>
       </c>
       <c r="K2">
-        <v>26600000</v>
+        <v>0.2</v>
       </c>
       <c r="L2">
-        <v>0.2</v>
+        <v>4.3</v>
       </c>
       <c r="M2">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="N2">
-        <v>4.5</v>
+        <v>0.83</v>
       </c>
       <c r="O2">
-        <v>0.83</v>
+        <v>1.5</v>
       </c>
       <c r="P2">
-        <v>1.5</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="Q2">
-        <v>7.5999999999999998E-2</v>
+        <v>1874</v>
       </c>
       <c r="R2">
-        <v>1874</v>
+        <v>0.1</v>
       </c>
       <c r="S2">
+        <v>0.85</v>
+      </c>
+      <c r="T2">
         <v>0.1</v>
       </c>
-      <c r="T2">
-        <v>0.85</v>
-      </c>
       <c r="U2">
-        <v>0.1</v>
+        <v>50</v>
       </c>
       <c r="V2">
-        <v>50</v>
+        <v>1500</v>
       </c>
       <c r="W2">
-        <v>1500</v>
+        <v>0.11</v>
       </c>
       <c r="X2">
-        <v>0.11</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="Y2">
-        <v>3.2000000000000001E-2</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="Z2">
-        <v>0.49199999999999999</v>
+        <v>0.1100000000000001</v>
       </c>
       <c r="AA2">
-        <v>0.1100000000000001</v>
+        <v>0.51041122056486954</v>
       </c>
       <c r="AB2">
-        <v>0.51041122056486954</v>
+        <v>3.3197477760316702E-2</v>
       </c>
       <c r="AC2">
-        <v>3.3197477760316702E-2</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE2">
         <v>1</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AG2">
-        <v>0.5</v>
+        <v>5000</v>
       </c>
       <c r="AH2">
-        <v>5000</v>
-      </c>
-      <c r="AI2">
         <v>10000</v>
       </c>
     </row>
@@ -1256,125 +1243,124 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>50</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="B2" t="s">
         <v>51</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
       </c>
       <c r="C2">
         <v>2018</v>
@@ -1383,96 +1369,93 @@
         <v>2030</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>18620000</v>
       </c>
       <c r="F2">
-        <v>18620000</v>
+        <v>0.17</v>
       </c>
       <c r="G2">
-        <v>0.17</v>
+        <v>2000</v>
       </c>
       <c r="H2">
-        <v>2000</v>
+        <v>0.16093946035233631</v>
       </c>
       <c r="I2">
-        <v>0.16093946035233631</v>
+        <v>30000000</v>
       </c>
       <c r="J2">
-        <v>30000000</v>
+        <v>26600000</v>
       </c>
       <c r="K2">
-        <v>26600000</v>
+        <v>0.2</v>
       </c>
       <c r="L2">
-        <v>0.2</v>
+        <v>4.3</v>
       </c>
       <c r="M2">
-        <v>4.3</v>
+        <v>4.5</v>
       </c>
       <c r="N2">
-        <v>4.5</v>
+        <v>0.83</v>
       </c>
       <c r="O2">
-        <v>0.83</v>
+        <v>1.5</v>
       </c>
       <c r="P2">
-        <v>1.5</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="Q2">
-        <v>7.5999999999999998E-2</v>
+        <v>1874</v>
       </c>
       <c r="R2">
-        <v>1874</v>
+        <v>0.1</v>
       </c>
       <c r="S2">
+        <v>0.85</v>
+      </c>
+      <c r="T2">
         <v>0.1</v>
       </c>
-      <c r="T2">
-        <v>0.85</v>
-      </c>
       <c r="U2">
-        <v>0.1</v>
+        <v>50</v>
       </c>
       <c r="V2">
-        <v>50</v>
+        <v>1500</v>
       </c>
       <c r="W2">
-        <v>1500</v>
+        <v>0.11</v>
       </c>
       <c r="X2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="Y2">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="Z2">
         <v>0.11</v>
       </c>
-      <c r="Y2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="Z2">
-        <v>0.49199999999999999</v>
-      </c>
       <c r="AA2">
-        <v>0.11</v>
+        <v>0.51041122056486954</v>
       </c>
       <c r="AB2">
-        <v>0.51041122056486954</v>
+        <v>3.3197477760316702E-2</v>
       </c>
       <c r="AC2">
-        <v>3.3197477760316702E-2</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE2">
         <v>1</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="AG2">
-        <v>0.5</v>
+        <v>5000</v>
       </c>
       <c r="AH2">
-        <v>5000</v>
-      </c>
-      <c r="AI2">
         <v>10000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final edits from Alex..
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -561,7 +561,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -645,7 +645,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="F2">
         <v>7.5999999999999998E-2</v>

</xml_diff>

<commit_message>
Updating cost values for Malawi
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="51">
   <si>
     <t>Scenario</t>
   </si>
@@ -110,15 +110,6 @@
   </si>
   <si>
     <t>NumPeoplePerHHUrban</t>
-  </si>
-  <si>
-    <t>DieselPriceLow</t>
-  </si>
-  <si>
-    <t>DieselPriceHigh</t>
-  </si>
-  <si>
-    <t>GridPrice</t>
   </si>
   <si>
     <t>GridCapacityInvestmentCost</t>
@@ -594,7 +585,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -644,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -677,7 +668,7 @@
         <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H1" t="s">
         <v>13</v>
@@ -772,10 +763,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,31 +784,28 @@
     <col min="11" max="11" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.140625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="12.7109375" style="2" customWidth="1"/>
-    <col min="29" max="29" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="49" width="9.140625" style="2" customWidth="1"/>
-    <col min="50" max="16384" width="9.140625" style="2"/>
+    <col min="14" max="14" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="46" width="9.140625" style="2" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -911,22 +899,13 @@
       <c r="AE1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C2" s="2">
         <v>2018</v>
@@ -959,57 +938,48 @@
         <v>4.5</v>
       </c>
       <c r="N2" s="2">
-        <v>0.83</v>
+        <v>1874</v>
       </c>
       <c r="O2" s="2">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="P2" s="2">
-        <v>7.5999999999999998E-2</v>
+        <v>0.85</v>
       </c>
       <c r="Q2" s="2">
-        <v>1874</v>
+        <v>0.1</v>
       </c>
       <c r="R2" s="2">
-        <v>0.1</v>
+        <v>50</v>
       </c>
       <c r="S2" s="2">
-        <v>0.85</v>
+        <v>1500</v>
       </c>
       <c r="T2" s="2">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="U2" s="2">
-        <v>50</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="V2" s="2">
-        <v>1500</v>
-      </c>
-      <c r="W2" s="2">
-        <v>0.11</v>
-      </c>
-      <c r="X2" s="2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="Y2" s="2">
         <v>0.49199999999999999</v>
       </c>
+      <c r="Z2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>1</v>
+      </c>
       <c r="AC2" s="2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AD2" s="2">
-        <v>1</v>
+        <v>5000</v>
       </c>
       <c r="AE2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>5000</v>
-      </c>
-      <c r="AH2" s="2">
         <v>10000</v>
       </c>
     </row>
@@ -1020,15 +990,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -1122,22 +1092,13 @@
       <c r="AE1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="B2" t="s">
         <v>48</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
       </c>
       <c r="C2">
         <v>2018</v>
@@ -1173,66 +1134,57 @@
         <v>4.5</v>
       </c>
       <c r="N2">
-        <v>0.83</v>
+        <v>1874</v>
       </c>
       <c r="O2">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="P2">
-        <v>7.5999999999999998E-2</v>
+        <v>0.85</v>
       </c>
       <c r="Q2">
-        <v>1874</v>
+        <v>0.1</v>
       </c>
       <c r="R2">
-        <v>0.1</v>
+        <v>50</v>
       </c>
       <c r="S2">
-        <v>0.85</v>
+        <v>1500</v>
       </c>
       <c r="T2">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="U2">
-        <v>50</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="V2">
-        <v>1500</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="W2">
-        <v>0.11</v>
+        <v>0.1100000000000001</v>
       </c>
       <c r="X2">
-        <v>3.2000000000000001E-2</v>
+        <v>0.51041122056486954</v>
       </c>
       <c r="Y2">
-        <v>0.49199999999999999</v>
+        <v>3.3197477760316702E-2</v>
       </c>
       <c r="Z2">
-        <v>0.1100000000000001</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>0.51041122056486954</v>
+        <v>1</v>
       </c>
       <c r="AB2">
-        <v>3.3197477760316702E-2</v>
+        <v>1</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <v>5000</v>
       </c>
       <c r="AE2">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>0.5</v>
-      </c>
-      <c r="AG2">
-        <v>5000</v>
-      </c>
-      <c r="AH2">
         <v>10000</v>
       </c>
     </row>
@@ -1243,15 +1195,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -1345,22 +1297,13 @@
       <c r="AE1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>47</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="B2" t="s">
         <v>48</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
       </c>
       <c r="C2">
         <v>2018</v>
@@ -1396,66 +1339,57 @@
         <v>4.5</v>
       </c>
       <c r="N2">
-        <v>0.83</v>
+        <v>1874</v>
       </c>
       <c r="O2">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="P2">
-        <v>7.5999999999999998E-2</v>
+        <v>0.85</v>
       </c>
       <c r="Q2">
-        <v>1874</v>
+        <v>0.1</v>
       </c>
       <c r="R2">
-        <v>0.1</v>
+        <v>50</v>
       </c>
       <c r="S2">
-        <v>0.85</v>
+        <v>1500</v>
       </c>
       <c r="T2">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="U2">
-        <v>50</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="V2">
-        <v>1500</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="W2">
         <v>0.11</v>
       </c>
       <c r="X2">
-        <v>3.2000000000000001E-2</v>
+        <v>0.51041122056486954</v>
       </c>
       <c r="Y2">
-        <v>0.49199999999999999</v>
+        <v>3.3197477760316702E-2</v>
       </c>
       <c r="Z2">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>0.51041122056486954</v>
+        <v>1</v>
       </c>
       <c r="AB2">
-        <v>3.3197477760316702E-2</v>
+        <v>1</v>
       </c>
       <c r="AC2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <v>5000</v>
       </c>
       <c r="AE2">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>0.5</v>
-      </c>
-      <c r="AG2">
-        <v>5000</v>
-      </c>
-      <c r="AH2">
         <v>10000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Grid Capacity limit fixed
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -635,7 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -765,7 +765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Specs changes for paper
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="SpecsDataCalib" sheetId="4" r:id="rId4"/>
     <sheet name="SpecsDataCalib1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1.2</v>
+        <v>0.94</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -729,7 +729,7 @@
         <v>0.8</v>
       </c>
       <c r="F3">
-        <v>8.4000000000000005E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="G3">
         <v>1.25</v>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,10 +923,10 @@
         <v>2000</v>
       </c>
       <c r="I2" s="2">
-        <v>30000000</v>
+        <v>26858617.899999999</v>
       </c>
       <c r="J2" s="2">
-        <v>26600000</v>
+        <v>26026616.100000001</v>
       </c>
       <c r="K2" s="2">
         <v>0.2</v>
@@ -993,10 +993,13 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -1119,10 +1122,10 @@
         <v>0.16093946035233631</v>
       </c>
       <c r="I2">
-        <v>30000000</v>
+        <v>26858617.899999999</v>
       </c>
       <c r="J2">
-        <v>26600000</v>
+        <v>26026616.100000001</v>
       </c>
       <c r="K2">
         <v>0.2</v>
@@ -1198,10 +1201,13 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -1324,10 +1330,10 @@
         <v>0.16093946035233631</v>
       </c>
       <c r="I2">
-        <v>30000000</v>
+        <v>26858617.899999999</v>
       </c>
       <c r="J2">
-        <v>26600000</v>
+        <v>26026616.100000001</v>
       </c>
       <c r="K2">
         <v>0.2</v>

</xml_diff>

<commit_message>
Revert "Merge branch 'cluster-algorithm-sunflower' of https://github.com/AndreasSahlberg/GEP-Working-dir into cluster-algorithm-sunflower"
This reverts commit 11ba9e07d9b7d462cc066f1131670ebf4be6fb69, reversing
changes made to 5c13efa5f653041b9d17fd82b0721271a4b9631d.
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="SpecsDataCalib" sheetId="4" r:id="rId4"/>
     <sheet name="SpecsDataCalib1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +703,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>0.94</v>
+        <v>1.2</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -729,7 +729,7 @@
         <v>0.8</v>
       </c>
       <c r="F3">
-        <v>9.5000000000000001E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="G3">
         <v>1.25</v>
@@ -765,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,10 +923,10 @@
         <v>2000</v>
       </c>
       <c r="I2" s="2">
-        <v>26858617.899999999</v>
+        <v>30000000</v>
       </c>
       <c r="J2" s="2">
-        <v>26026616.100000001</v>
+        <v>26600000</v>
       </c>
       <c r="K2" s="2">
         <v>0.2</v>
@@ -993,13 +993,10 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -1122,10 +1119,10 @@
         <v>0.16093946035233631</v>
       </c>
       <c r="I2">
-        <v>26858617.899999999</v>
+        <v>30000000</v>
       </c>
       <c r="J2">
-        <v>26026616.100000001</v>
+        <v>26600000</v>
       </c>
       <c r="K2">
         <v>0.2</v>
@@ -1201,13 +1198,10 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -1330,10 +1324,10 @@
         <v>0.16093946035233631</v>
       </c>
       <c r="I2">
-        <v>26858617.899999999</v>
+        <v>30000000</v>
       </c>
       <c r="J2">
-        <v>26026616.100000001</v>
+        <v>26600000</v>
       </c>
       <c r="K2">
         <v>0.2</v>

</xml_diff>

<commit_message>
Minor PV cost updates
</commit_message>
<xml_diff>
--- a/specs_mw_one_scenario.xlsx
+++ b/specs_mw_one_scenario.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\TEST RUNS GEP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adm.esa\Documents\GitHub\GEP-Working-dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -560,20 +560,20 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -640,23 +640,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>8</v>
       </c>
@@ -691,7 +691,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -729,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -749,7 +749,7 @@
         <v>109</v>
       </c>
       <c r="G3">
-        <v>8.4000000000000005E-2</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="H3">
         <v>1.25</v>
@@ -767,7 +767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -776,6 +776,9 @@
       </c>
       <c r="D4">
         <v>6</v>
+      </c>
+      <c r="H4">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>
@@ -792,43 +795,43 @@
       <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.109375" style="2" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" style="2" customWidth="1"/>
-    <col min="26" max="26" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="46" width="9.109375" style="2" customWidth="1"/>
-    <col min="47" max="16384" width="9.109375" style="2"/>
+    <col min="32" max="46" width="9.140625" style="2" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -923,7 +926,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -1015,13 +1018,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
@@ -1116,7 +1119,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -1142,10 +1145,10 @@
         <v>0.16093946035233631</v>
       </c>
       <c r="I2">
-        <v>30000000</v>
+        <v>26858617.899999999</v>
       </c>
       <c r="J2">
-        <v>26600000</v>
+        <v>26026616.100000001</v>
       </c>
       <c r="K2">
         <v>0.2</v>

</xml_diff>